<commit_message>
prep for urban water consumed plus Owen working
</commit_message>
<xml_diff>
--- a/Willamette Basin water budget summary 2-22-15.xlsx
+++ b/Willamette Basin water budget summary 2-22-15.xlsx
@@ -589,11 +589,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145274368"/>
-        <c:axId val="70156288"/>
+        <c:axId val="128696320"/>
+        <c:axId val="128697856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145274368"/>
+        <c:axId val="128696320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70156288"/>
+        <c:crossAx val="128697856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70156288"/>
+        <c:axId val="128697856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145274368"/>
+        <c:crossAx val="128696320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1195,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O36"/>
+  <dimension ref="A2:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,6 +2544,71 @@
         <v>2.9381187190000002</v>
       </c>
     </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1">
+        <f>D28-D36-D32-D30-D29</f>
+        <v>7.1647144529999984</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" ref="E38:O38" si="0">E28-E36-E32-E30-E29</f>
+        <v>12.680443746</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7676039969999993</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.28469918699999996</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60946453699999892</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.5092733900000006</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.488388967000001</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="0"/>
+        <v>-5.2051209079999996</v>
+      </c>
+      <c r="L38" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.692755461</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.0201018929999996</v>
+      </c>
+      <c r="N38" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.1432940800000004</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32187515599999966</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>